<commit_message>
added new daily measurements
</commit_message>
<xml_diff>
--- a/data/environmental/daily_measurements.xlsx
+++ b/data/environmental/daily_measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/environmental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AC7677-5001-7E46-AC7B-535E84995FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0680A9-74FB-9349-99F6-5AD2564F1D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17440" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>pH.mV</t>
   </si>
@@ -65,13 +65,13 @@
     <t>notes</t>
   </si>
   <si>
-    <t>water_table</t>
-  </si>
-  <si>
     <t>rainy, cloudy</t>
   </si>
   <si>
-    <t>blue_tank</t>
+    <t>water table</t>
+  </si>
+  <si>
+    <t>blue tank</t>
   </si>
 </sst>
 </file>
@@ -107,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5716CA15-A063-CD4A-965E-FFCB3C4243EA}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,7 +473,7 @@
         <v>1500</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>-70.900000000000006</v>
@@ -490,7 +491,7 @@
         <v>20231105</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -519,7 +520,65 @@
         <v>20231105</v>
       </c>
       <c r="I3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45236</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.50138888888888888</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
+      </c>
+      <c r="D4">
+        <v>-69.900000000000006</v>
+      </c>
+      <c r="E4">
+        <v>28.36</v>
+      </c>
+      <c r="F4">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="G4">
+        <v>376</v>
+      </c>
+      <c r="H4">
+        <v>20231105</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45236</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>-69.3</v>
+      </c>
+      <c r="E5">
+        <v>28.8</v>
+      </c>
+      <c r="F5">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="G5">
+        <v>517</v>
+      </c>
+      <c r="H5">
+        <v>20231105</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated daily measurement data
</commit_message>
<xml_diff>
--- a/data/environmental/daily_measurements.xlsx
+++ b/data/environmental/daily_measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloegilligan/Desktop/PutnamLab/Repositories /moorea_symbiotic_exchange_2023/data/environmental/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/environmental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731A9066-F943-4C45-9CD8-8AEE2C145714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB240B1-9449-8F4D-BD14-587AC6B21415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13100" yWindow="760" windowWidth="18740" windowHeight="17440" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
+    <workbookView xWindow="11500" yWindow="760" windowWidth="18740" windowHeight="17440" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="19">
   <si>
     <t>pH.mV</t>
   </si>
@@ -449,7 +449,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,8 +1172,8 @@
       <c r="F25">
         <v>36.049999999999997</v>
       </c>
-      <c r="G25" t="s">
-        <v>14</v>
+      <c r="G25">
+        <v>580</v>
       </c>
       <c r="H25">
         <v>20231105</v>
@@ -1201,8 +1201,8 @@
       <c r="F26">
         <v>36.06</v>
       </c>
-      <c r="G26" t="s">
-        <v>14</v>
+      <c r="G26">
+        <v>582</v>
       </c>
       <c r="H26">
         <v>20231105</v>
@@ -1230,8 +1230,8 @@
       <c r="F27">
         <v>36.21</v>
       </c>
-      <c r="G27" t="s">
-        <v>14</v>
+      <c r="G27">
+        <v>590</v>
       </c>
       <c r="H27">
         <v>20231105</v>

</xml_diff>